<commit_message>
Updated STM32 to reflect build.  Updated BOM and Schematic
</commit_message>
<xml_diff>
--- a/1u_panel/doc/BOM/1u_panel.xlsx
+++ b/1u_panel/doc/BOM/1u_panel.xlsx
@@ -536,13 +536,13 @@
     <t xml:space="preserve">U6</t>
   </si>
   <si>
-    <t xml:space="preserve">STM32F042K6T6</t>
+    <t xml:space="preserve">STM32F042K6T7</t>
   </si>
   <si>
     <t xml:space="preserve">Cortex®-M0 STM32F0 IC 32-Bit 48Mhz 32KB 32-LQFP (7x7)</t>
   </si>
   <si>
-    <t xml:space="preserve">497-14647-ND</t>
+    <t xml:space="preserve">STM32F042K6T7-ND</t>
   </si>
   <si>
     <t xml:space="preserve">X1</t>
@@ -567,11 +567,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -601,6 +602,13 @@
       <color rgb="FF000000"/>
       <name val="Sans"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -646,7 +654,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -657,6 +665,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -679,7 +691,7 @@
   <dimension ref="A1:IP41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H43" activeCellId="0" sqref="H43"/>
+      <selection pane="topLeft" activeCell="I40" activeCellId="0" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -687,74 +699,74 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="68.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="187" min="10" style="1" width="10.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="188" min="188" style="1" width="9.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="188" min="188" style="1" width="9.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="189" min="189" style="1" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="190" min="190" style="1" width="9.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="191" min="191" style="1" width="4.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="192" min="192" style="1" width="42.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="193" min="193" style="1" width="6.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="194" min="194" style="1" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="194" min="194" style="1" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="195" min="195" style="1" width="4.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="196" min="196" style="1" width="8.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="197" min="197" style="1" width="6.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="198" min="198" style="1" width="9.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="198" min="198" style="1" width="9.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="199" min="199" style="1" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="200" min="200" style="1" width="9.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="201" min="201" style="1" width="4.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="202" min="202" style="1" width="42.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="203" min="203" style="1" width="6.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="204" min="204" style="1" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="204" min="204" style="1" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="205" min="205" style="1" width="4.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="206" min="206" style="1" width="8.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="207" min="207" style="1" width="6.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="208" min="208" style="1" width="9.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="208" min="208" style="1" width="9.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="209" min="209" style="1" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="210" min="210" style="1" width="9.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="211" min="211" style="1" width="4.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="212" min="212" style="1" width="42.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="213" min="213" style="1" width="6.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="214" min="214" style="1" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="214" min="214" style="1" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="215" min="215" style="1" width="4.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="216" min="216" style="1" width="8.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="217" min="217" style="1" width="6.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="218" min="218" style="1" width="9.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="218" min="218" style="1" width="9.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="219" min="219" style="1" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="220" min="220" style="1" width="9.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="221" min="221" style="1" width="4.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="222" min="222" style="1" width="42.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="223" min="223" style="1" width="6.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="224" min="224" style="1" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="224" min="224" style="1" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="225" min="225" style="1" width="4.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="226" min="226" style="1" width="8.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="227" min="227" style="1" width="6.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="228" min="228" style="1" width="9.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="228" min="228" style="1" width="9.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="229" min="229" style="1" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="230" min="230" style="1" width="9.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="231" min="231" style="1" width="4.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="232" min="232" style="1" width="42.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="233" min="233" style="1" width="6.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="234" min="234" style="1" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="234" min="234" style="1" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="235" min="235" style="1" width="4.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="236" min="236" style="1" width="8.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="237" min="237" style="1" width="6.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="238" min="238" style="1" width="9.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="238" min="238" style="1" width="9.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="239" min="239" style="1" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="240" min="240" style="1" width="9.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="241" min="241" style="1" width="4.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="242" min="242" style="1" width="42.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="243" min="243" style="1" width="6.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="244" min="244" style="1" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="244" min="244" style="1" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="245" min="245" style="1" width="4.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="246" min="246" style="1" width="8.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="247" min="247" style="1" width="6.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="248" min="248" style="1" width="9.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="248" min="248" style="1" width="9.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="249" min="249" style="1" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="250" min="250" style="1" width="9.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="251" style="1" width="10.45"/>
@@ -3496,7 +3508,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>1</v>
       </c>
@@ -3521,7 +3533,7 @@
       <c r="H40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="I40" s="3" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3557,7 +3569,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="atEnd" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>